<commit_message>
pengguna online - view & edit
</commit_message>
<xml_diff>
--- a/Data Files/TestData/NexCare/Pengaturan/Flow Chatbot/Flow Chatbot - add.xlsx
+++ b/Data Files/TestData/NexCare/Pengaturan/Flow Chatbot/Flow Chatbot - add.xlsx
@@ -14,13 +14,14 @@
     <sheet name="pesanerror" sheetId="5" r:id="rId5"/>
     <sheet name="pesantimeout" sheetId="6" r:id="rId6"/>
     <sheet name="pesanbuattiket" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="152">
   <si>
     <t>TD</t>
   </si>
@@ -37,12 +38,18 @@
     <t>Pesan otomatis</t>
   </si>
   <si>
+    <t>Judul Template</t>
+  </si>
+  <si>
     <t>List Jawaban</t>
   </si>
   <si>
     <t>URL Link</t>
   </si>
   <si>
+    <t>KMS List</t>
+  </si>
+  <si>
     <t>Batas Waktu Pesan</t>
   </si>
   <si>
@@ -58,6 +65,9 @@
     <t>expected resut</t>
   </si>
   <si>
+    <t>Toggle</t>
+  </si>
+  <si>
     <t>TDG221501</t>
   </si>
   <si>
@@ -293,6 +303,387 @@
   </si>
   <si>
     <t>google.com</t>
+  </si>
+  <si>
+    <t>TDG221541</t>
+  </si>
+  <si>
+    <t>qna</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ini pesan question n answer ola</t>
+    </r>
+  </si>
+  <si>
+    <t>Pertanyaan1</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>TDG221542</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sdad~`!@#$%^&amp;*()_+-={}[]|&lt;,&gt;.?/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pertanyaan2</t>
+    </r>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>TDG221543</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pertanyaan3</t>
+    </r>
+  </si>
+  <si>
+    <t>gromart,nexchief,nexpos</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>TDG221544</t>
+  </si>
+  <si>
+    <t>nexchief</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ini pertanyaan pertama</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pertanyaan4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>nexcare,nextrac</t>
+    </r>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>TDG221545</t>
+  </si>
+  <si>
+    <t>nexcare</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ini pertanyaan kedua</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pertanyaan5</t>
+    </r>
+  </si>
+  <si>
+    <t>TDG221546</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ini pertanyaan ketiga</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pertanyaan6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>grochat,grolog</t>
+    </r>
+  </si>
+  <si>
+    <t>Mutasi adjust stock HA</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>TDG221547</t>
+  </si>
+  <si>
+    <t>TDG221548</t>
+  </si>
+  <si>
+    <t>nextrac</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ini pertanyaan ola</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ini jawaban1,ini jawaban2</t>
+    </r>
+  </si>
+  <si>
+    <t>TDG221549</t>
+  </si>
+  <si>
+    <t>nexpos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ini jawaban13,ini jawaban23</t>
+    </r>
+  </si>
+  <si>
+    <t>TDG221550</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ini ola</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PertanyaanA</t>
+    </r>
+  </si>
+  <si>
+    <t>TDG221551</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>elit eget gravida cum sociis natoque penatibus et magnis dis parturient montes nascetur ridiculus mus mauris vitae ultricies leo integer malesuada nunc vel risus commodo viverra maecenas accumsan lacus vel facilisis volutpat est velit egestas dui id ornare arcu odio ut sem nulla pharetra diam sitamet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PertanyaanB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Apakah jawaban ini membantu?</t>
+    </r>
+  </si>
+  <si>
+    <t>TDG221552</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ini link create ticket</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PertanyaanC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>qe</t>
+    </r>
+  </si>
+  <si>
+    <t>TDG221553</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PertanyaanD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>elit eget gravida cum sociis natoque penatibus etma</t>
+    </r>
+  </si>
+  <si>
+    <t>TDG221554</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PertanyaanE</t>
+    </r>
+  </si>
+  <si>
+    <t>ht://www.google.com/</t>
   </si>
   <si>
     <t>Link URL</t>
@@ -342,15 +733,15 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -520,6 +911,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -557,12 +954,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,7 +1228,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -861,16 +1252,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -879,16 +1270,16 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -961,42 +1352,54 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1008,9 +1411,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
@@ -1334,10 +1760,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1346,14 +1772,15 @@
     <col min="2" max="2" width="7.28571428571429" customWidth="1"/>
     <col min="3" max="3" width="17.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="30.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="48.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="32.4285714285714" customWidth="1"/>
-    <col min="7" max="9" width="24.1428571428571" customWidth="1"/>
-    <col min="10" max="10" width="15.4285714285714" customWidth="1"/>
-    <col min="12" max="12" width="59.8571428571429" customWidth="1"/>
+    <col min="5" max="6" width="48.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="32.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="29.7428571428571" customWidth="1"/>
+    <col min="9" max="11" width="24.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="15.4285714285714" customWidth="1"/>
+    <col min="14" max="14" width="59.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,911 +1811,1421 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="M1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="10"/>
+        <v>18</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="3"/>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="3"/>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="3"/>
-      <c r="K5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" ht="90" spans="1:11">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="3"/>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" ht="90" spans="1:13">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="3"/>
-      <c r="K6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="3"/>
+      <c r="M6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
       <c r="E9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="7">
-        <v>1</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="13">
         <v>2</v>
       </c>
-      <c r="K10" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="M10" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>42</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="M11" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>21</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="M12" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="M13" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="K14" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="F14" s="23"/>
+      <c r="M14" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" ht="90" spans="1:11">
+        <v>26</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="M15" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" ht="90" spans="1:13">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="M16" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="F17" s="14"/>
+      <c r="M17" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="M18" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="M19" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="23"/>
+      <c r="M20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="M21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" ht="90" spans="1:13">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="24"/>
+      <c r="M22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="M23" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="M24" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="23"/>
+      <c r="J25" s="3">
+        <v>65</v>
+      </c>
+      <c r="K25" s="3">
+        <v>286</v>
+      </c>
+      <c r="M25" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="23"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="M26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="M27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" ht="90" spans="1:13">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="M28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="14"/>
+      <c r="J29" s="7">
+        <v>78</v>
+      </c>
+      <c r="K29" s="7">
+        <v>65</v>
+      </c>
+      <c r="M29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="J30" s="7">
+        <v>370</v>
+      </c>
+      <c r="K30" s="7">
+        <v>609</v>
+      </c>
+      <c r="M30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="J31" s="7">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="K20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" ht="90" spans="1:11">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="K23" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
+      <c r="K31" s="7">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="K24" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="s">
+      <c r="M31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
         <v>60</v>
       </c>
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="3">
-        <v>65</v>
-      </c>
-      <c r="I25" s="3">
-        <v>286</v>
-      </c>
-      <c r="K25" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="K26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="K27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" ht="90" spans="1:11">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="K28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="H29" s="10">
-        <v>78</v>
-      </c>
-      <c r="I29" s="10">
-        <v>65</v>
-      </c>
-      <c r="K29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" s="10">
-        <v>370</v>
-      </c>
-      <c r="I30" s="10">
-        <v>609</v>
-      </c>
-      <c r="K30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" s="10">
-        <v>13</v>
-      </c>
-      <c r="I31" s="10">
-        <v>59</v>
-      </c>
-      <c r="K31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="5">
+      <c r="D32" s="23"/>
+      <c r="E32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="10">
         <v>60</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>180</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" s="28"/>
+      <c r="M32" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="F33" s="3"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="5"/>
-      <c r="I33"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
         <v>72</v>
-      </c>
-      <c r="B35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" t="s">
-        <v>69</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="11"/>
+      <c r="L35" s="11">
+        <v>2</v>
+      </c>
+      <c r="M35" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="12"/>
+      <c r="M36" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="7"/>
-      <c r="J35" s="7">
-        <v>2</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="4"/>
-      <c r="K36" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H37" s="9"/>
-      <c r="J37" s="9">
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I37" s="6"/>
+      <c r="J37" s="13"/>
+      <c r="L37" s="13">
         <v>3</v>
       </c>
-      <c r="K37" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="M37" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="K38" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" ht="90" spans="1:11">
+        <v>26</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="14"/>
+      <c r="M38" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" ht="90" spans="1:13">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="14"/>
+      <c r="L39" s="13">
+        <v>4</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H40" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G39" s="10"/>
-      <c r="H39"/>
-      <c r="J39">
-        <v>4</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F40" s="10" t="s">
+      <c r="I40" s="16"/>
+      <c r="J40" s="17"/>
+      <c r="L40" s="17">
+        <v>5</v>
+      </c>
+      <c r="M40" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="16"/>
+      <c r="J41" s="17"/>
+      <c r="L41" s="17">
+        <v>5</v>
+      </c>
+      <c r="M41" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G40" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H40" s="13"/>
-      <c r="J40" s="13">
-        <v>5</v>
-      </c>
-      <c r="K40" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H41" s="13"/>
-      <c r="J41" s="13">
+      <c r="H42" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I42" s="16"/>
+      <c r="J42" s="17"/>
+      <c r="L42" s="17">
         <v>6</v>
       </c>
-      <c r="K41" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="10" t="s">
+      <c r="M42" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="29"/>
+      <c r="M43" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="O43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="26"/>
+      <c r="E44" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F44" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="29"/>
+      <c r="M44" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="O44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H45" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="G42" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H42" s="13"/>
-      <c r="J42" s="13">
-        <v>7</v>
-      </c>
-      <c r="K42" s="11" t="s">
-        <v>20</v>
+      <c r="I45" s="30"/>
+      <c r="L45" t="s">
+        <v>106</v>
+      </c>
+      <c r="M45" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="O45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="H46" s="26"/>
+      <c r="I46" s="29"/>
+      <c r="L46" t="s">
+        <v>112</v>
+      </c>
+      <c r="M46" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="O46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="29"/>
+      <c r="M47" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="O47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="H48" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I48" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="L48" t="s">
+        <v>112</v>
+      </c>
+      <c r="M48" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="O48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" customFormat="1" spans="1:13">
+      <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="31"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" customFormat="1" spans="1:13">
+      <c r="A50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="H50" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I50" s="32"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50" t="s">
+        <v>112</v>
+      </c>
+      <c r="M50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" customFormat="1" spans="1:13">
+      <c r="A51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="H51" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I51" s="32"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51" t="s">
+        <v>112</v>
+      </c>
+      <c r="M51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" customFormat="1" spans="1:13">
+      <c r="A52" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="29"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" customFormat="1" ht="90" spans="1:13">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="H53" s="26"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" customFormat="1" spans="1:13">
+      <c r="A54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F54" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="H54" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I54" s="32"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" customFormat="1" ht="30" spans="1:13">
+      <c r="A55" t="s">
+        <v>143</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F55" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="H55" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I55" s="32"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" customFormat="1" ht="30" spans="1:13">
+      <c r="A56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="H56" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="I56" s="32"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G10" r:id="rId1" display="https://www.google.com" tooltip="https://www.google.com"/>
-    <hyperlink ref="G37" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
-    <hyperlink ref="G40" r:id="rId2" display="https://www.google.com/"/>
-    <hyperlink ref="G41" r:id="rId2" display="https://www.google.com/"/>
-    <hyperlink ref="G42" r:id="rId3" display="google.com"/>
+    <hyperlink ref="H10" r:id="rId1" display="https://www.google.com" tooltip="https://www.google.com"/>
+    <hyperlink ref="H37" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H40" r:id="rId2" display="https://www.google.com/"/>
+    <hyperlink ref="H41" r:id="rId2" display="https://www.google.com/"/>
+    <hyperlink ref="H42" r:id="rId3" display="google.com"/>
+    <hyperlink ref="H50" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H51" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H54" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H55" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H56" r:id="rId2" display="ht://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H45" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H48" r:id="rId2" display="https://www.google.com/" tooltip="https://www.google.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2317,20 +3254,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2338,91 +3275,91 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="C4" s="20"/>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2452,29 +3389,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
+      <c r="D1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -2482,92 +3419,92 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="20" t="s">
-        <v>16</v>
+      <c r="F2" s="10"/>
+      <c r="G2" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="20" t="s">
-        <v>16</v>
+      <c r="F3" s="10"/>
+      <c r="G3" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="7">
+        <v>150</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>16</v>
+      <c r="G4" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="9">
+        <v>82</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="13">
         <v>2</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>16</v>
+      <c r="G5" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2599,20 +3536,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>93</v>
+      <c r="D1" s="19" t="s">
+        <v>151</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2620,128 +3557,128 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="20" t="s">
-        <v>16</v>
+      <c r="E2" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="20" t="s">
-        <v>16</v>
+      <c r="E3" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="20" t="s">
-        <v>20</v>
+      <c r="E5" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="20" t="s">
-        <v>20</v>
+      <c r="E6" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="135" spans="1:6">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2770,20 +3707,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>10</v>
+      <c r="D1" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -2791,91 +3728,91 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>16</v>
+        <v>53</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2905,26 +3842,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>10</v>
       </c>
+      <c r="F1" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -2932,51 +3869,51 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="20" t="s">
-        <v>16</v>
+      <c r="F2" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" ht="30" spans="1:8">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="20" t="s">
-        <v>16</v>
+      <c r="F3" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D4" s="3">
         <v>65</v>
@@ -2984,139 +3921,139 @@
       <c r="E4" s="3">
         <v>286</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>16</v>
+      <c r="F4" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" ht="165" spans="1:8">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7">
         <v>78</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="10">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="7">
         <v>370</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>609</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="7">
         <v>13</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="10">
-        <v>13</v>
-      </c>
-      <c r="E10" s="10">
+      <c r="E10" s="7">
         <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3147,32 +4084,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
+      <c r="F1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -3180,246 +4117,246 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="20" t="s">
-        <v>16</v>
+      <c r="G2" s="10"/>
+      <c r="H2" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="20" t="s">
-        <v>16</v>
+      <c r="G3" s="10"/>
+      <c r="H3" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="7">
+      <c r="G4" s="11">
         <v>2</v>
       </c>
-      <c r="H4" s="20" t="s">
-        <v>16</v>
+      <c r="H4" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="4"/>
-      <c r="H5" s="20" t="s">
-        <v>16</v>
+      <c r="H5" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="9">
+        <v>82</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="13">
         <v>3</v>
       </c>
-      <c r="H6" s="20" t="s">
-        <v>16</v>
+      <c r="H6" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="H7" s="11" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" ht="135" spans="1:10">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="G8">
         <v>4</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>20</v>
+      <c r="H8" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="13">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="17">
         <v>5</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>20</v>
+      <c r="H9" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="E10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="17">
         <v>6</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>20</v>
+      <c r="H10" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="13">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="17">
         <v>7</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>20</v>
+      <c r="H11" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3432,4 +4369,374 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="7.28571428571429" customWidth="1"/>
+    <col min="3" max="3" width="17.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="30.7142857142857" customWidth="1"/>
+    <col min="5" max="6" width="48.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="32.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="29.7428571428571" customWidth="1"/>
+    <col min="9" max="11" width="24.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="15.4285714285714" customWidth="1"/>
+    <col min="13" max="13" width="9"/>
+    <col min="14" max="14" width="59.8571428571429" customWidth="1"/>
+    <col min="15" max="15" width="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" spans="1:13">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="10"/>
+      <c r="K2"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:13">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="10"/>
+      <c r="K3"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:13">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="11"/>
+      <c r="K4"/>
+      <c r="L4" s="11">
+        <v>2</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:13">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="12"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:13">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="13"/>
+      <c r="K6"/>
+      <c r="L6" s="13">
+        <v>3</v>
+      </c>
+      <c r="M6" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:13">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="14"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" ht="90" spans="1:13">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="14"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8" s="13">
+        <v>4</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" spans="1:13">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9"/>
+      <c r="L9" s="17">
+        <v>5</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" spans="1:13">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="17"/>
+      <c r="K10"/>
+      <c r="L10" s="17">
+        <v>5</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="1:13">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11"/>
+      <c r="L11" s="17">
+        <v>6</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" display="https://www.google.com/" tooltip="https://www.google.com/"/>
+    <hyperlink ref="H9" r:id="rId1" display="https://www.google.com/"/>
+    <hyperlink ref="H10" r:id="rId1" display="https://www.google.com/"/>
+    <hyperlink ref="H11" r:id="rId2" display="google.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>